<commit_message>
Name of variables iService, iMontecarlo and associatedElements changed. Switches notebook adapted.
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/switches_v2/network.xlsx
+++ b/jupyter_notebooks/file/input/switches_v2/network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\jupyter_notebooks\file\input\switches_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF77A6F-9E2E-4FDA-8AE0-CB641A59AA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBFE44E-6253-4DD9-BCFB-C5951BF95CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{D3DCB828-FBC6-4B5F-B916-8216FBF30931}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{D3DCB828-FBC6-4B5F-B916-8216FBF30931}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="191">
   <si>
     <t>name</t>
   </si>
@@ -569,9 +569,6 @@
     <t>swb2-tr1</t>
   </si>
   <si>
-    <t>swb7-l8</t>
-  </si>
-  <si>
     <t>swb2-l1</t>
   </si>
   <si>
@@ -620,10 +617,10 @@
     <t>line7, line8, line9, load9</t>
   </si>
   <si>
-    <t>line7, line8, line9, load9, g18</t>
-  </si>
-  <si>
     <t>swb18-l19</t>
+  </si>
+  <si>
+    <t>swb8-l7</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1499,7 @@
         <v>138</v>
       </c>
       <c r="J1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -5305,7 +5302,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20">
         <v>110</v>
@@ -5339,7 +5336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -5400,7 +5397,7 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M1" t="s">
         <v>33</v>
@@ -5711,7 +5708,7 @@
         <v>45</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L10" s="2"/>
       <c r="O10">
@@ -5847,7 +5844,7 @@
         <v>45</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>105</v>
@@ -5971,13 +5968,13 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
         <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18">
         <v>27</v>
@@ -6004,7 +6001,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B19" t="s">
         <v>108</v>
@@ -6047,8 +6044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B254C9-296C-496E-B9D1-44F56B1564BD}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6082,10 +6079,10 @@
         <v>164</v>
       </c>
       <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
         <v>186</v>
-      </c>
-      <c r="I1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6123,7 +6120,7 @@
         <v>105</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>180</v>
+        <v>121</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -6159,14 +6156,14 @@
         <v>171</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
         <v>109</v>
@@ -6181,13 +6178,13 @@
         <v>105</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -6208,7 +6205,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -6223,13 +6220,13 @@
         <v>105</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -6244,13 +6241,13 @@
         <v>105</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -6265,28 +6262,28 @@
         <v>105</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
         <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
         <v>169</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>105</v>
@@ -6378,7 +6375,7 @@
         <v>158</v>
       </c>
       <c r="R1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -6623,10 +6620,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10">
         <v>5.6211919330659503</v>
@@ -6771,7 +6768,7 @@
         <v>158</v>
       </c>
       <c r="AA1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>